<commit_message>
Allineamento indicatori retail per le librerie
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/53_Inst_Analysis_Unit_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/53_Inst_Analysis_Unit_RETAIL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16638" yWindow="0" windowWidth="18318" windowHeight="7380"/>
+    <workbookView xWindow="16635" yWindow="0" windowWidth="18315" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_Unit" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="208">
   <si>
     <t>Analysis_Unit</t>
   </si>
@@ -539,12 +539,6 @@
     <t>COUNTERPARTY_RETAIL_IND_53</t>
   </si>
   <si>
-    <t>COUNTERPARTY_RETAIL_IND_54</t>
-  </si>
-  <si>
-    <t>COUNTERPARTY_RETAIL_IND_55</t>
-  </si>
-  <si>
     <t>COUNTERPARTY_RETAIL_IND_60</t>
   </si>
   <si>
@@ -596,12 +590,6 @@
     <t>RETAIL_IND_53</t>
   </si>
   <si>
-    <t>RETAIL_IND_54</t>
-  </si>
-  <si>
-    <t>RETAIL_IND_55</t>
-  </si>
-  <si>
     <t>RETAIL_IND_60</t>
   </si>
   <si>
@@ -645,6 +633,42 @@
   </si>
   <si>
     <t>RETAIL_IND_87</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_14</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_14</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_50</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_51</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_50</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_51</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_200</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_200</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_150</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_151</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_150</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_151</t>
   </si>
 </sst>
 </file>
@@ -1268,19 +1292,19 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.83984375" customWidth="1"/>
-    <col min="8" max="8" width="30.26171875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1317,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1357,21 +1381,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1381,7 +1405,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1401,7 +1425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1418,7 +1442,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1435,7 +1459,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1486,7 +1510,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1527,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1520,7 +1544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1537,7 +1561,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1554,7 +1578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1595,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1588,1245 +1612,1313 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>49</v>
       </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>53</v>
       </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
         <v>162</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>162</v>
       </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" t="s">
-        <v>163</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" t="s">
-        <v>164</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" t="s">
-        <v>165</v>
-      </c>
-      <c r="E29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" t="s">
-        <v>166</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" t="s">
-        <v>167</v>
-      </c>
-      <c r="E31" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" t="s">
-        <v>169</v>
-      </c>
-      <c r="E33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" t="s">
-        <v>170</v>
-      </c>
-      <c r="E34" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>171</v>
-      </c>
-      <c r="C35" t="s">
-        <v>171</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" t="s">
-        <v>172</v>
-      </c>
-      <c r="C36" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" t="s">
-        <v>173</v>
-      </c>
-      <c r="C37" t="s">
-        <v>173</v>
-      </c>
-      <c r="E37" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" t="s">
-        <v>174</v>
-      </c>
-      <c r="E38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" t="s">
-        <v>176</v>
-      </c>
-      <c r="C40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" t="s">
-        <v>177</v>
-      </c>
-      <c r="C41" t="s">
-        <v>177</v>
-      </c>
-      <c r="E41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" t="s">
-        <v>178</v>
-      </c>
-      <c r="C42" t="s">
-        <v>178</v>
-      </c>
-      <c r="E42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" t="s">
-        <v>179</v>
-      </c>
-      <c r="C43" t="s">
-        <v>179</v>
-      </c>
-      <c r="E43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" t="s">
-        <v>180</v>
-      </c>
-      <c r="C44" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
         <v>78</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>78</v>
       </c>
-      <c r="E45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
         <v>79</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>79</v>
       </c>
-      <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
         <v>80</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>80</v>
       </c>
-      <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
         <v>81</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>81</v>
       </c>
-      <c r="E48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
         <v>82</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>82</v>
       </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
         <v>83</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>83</v>
       </c>
-      <c r="E50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
         <v>84</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>84</v>
       </c>
-      <c r="E51" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
         <v>85</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>85</v>
       </c>
-      <c r="E52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
         <v>86</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>86</v>
       </c>
-      <c r="E53" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
         <v>87</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>87</v>
       </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
         <v>88</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>88</v>
       </c>
-      <c r="E55" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
-        <v>20</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
         <v>89</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>89</v>
       </c>
-      <c r="E56" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
         <v>90</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>90</v>
       </c>
-      <c r="E57" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
-        <v>20</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
         <v>91</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>91</v>
       </c>
-      <c r="E58" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
         <v>92</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>92</v>
       </c>
-      <c r="E59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
         <v>93</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>93</v>
       </c>
-      <c r="E60" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
-        <v>20</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
         <v>94</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>94</v>
       </c>
-      <c r="E61" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>20</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
         <v>95</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>95</v>
       </c>
-      <c r="E62" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>20</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
         <v>96</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>96</v>
       </c>
-      <c r="E63" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
-        <v>20</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
         <v>97</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>97</v>
       </c>
-      <c r="E64" t="s">
-        <v>26</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
         <v>98</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>98</v>
       </c>
-      <c r="E65" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
         <v>99</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C68" t="s">
         <v>99</v>
       </c>
-      <c r="E66" t="s">
-        <v>26</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" t="s">
-        <v>20</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
         <v>100</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>100</v>
       </c>
-      <c r="E67" t="s">
-        <v>26</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
         <v>101</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
         <v>101</v>
       </c>
-      <c r="E68" t="s">
-        <v>26</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
-        <v>20</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
         <v>102</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>102</v>
       </c>
-      <c r="E69" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="s">
-        <v>20</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
         <v>103</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>103</v>
       </c>
-      <c r="E70" t="s">
-        <v>26</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E72" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B71" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
         <v>104</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>104</v>
       </c>
-      <c r="E71" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="s">
-        <v>20</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
         <v>105</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>105</v>
       </c>
-      <c r="E72" t="s">
-        <v>26</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E74" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
-        <v>20</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
         <v>106</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>106</v>
       </c>
-      <c r="E73" t="s">
-        <v>26</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="s">
-        <v>20</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
         <v>107</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>107</v>
       </c>
-      <c r="E74" t="s">
-        <v>26</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E76" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
         <v>108</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>108</v>
       </c>
-      <c r="E75" t="s">
-        <v>26</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="E77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="s">
-        <v>20</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
         <v>109</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C78" t="s">
         <v>109</v>
       </c>
-      <c r="E76" t="s">
-        <v>26</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E78" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="s">
-        <v>20</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
         <v>110</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>110</v>
       </c>
-      <c r="E77" t="s">
-        <v>26</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+      <c r="F79" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
-        <v>20</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
         <v>111</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C80" t="s">
         <v>111</v>
       </c>
-      <c r="E78" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+      <c r="F80" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="s">
-        <v>20</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
         <v>112</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C81" t="s">
         <v>112</v>
       </c>
-      <c r="E79" t="s">
-        <v>26</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" t="s">
-        <v>20</v>
-      </c>
-      <c r="B80" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
         <v>113</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C82" t="s">
         <v>113</v>
       </c>
-      <c r="E80" t="s">
-        <v>26</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E82" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" t="s">
-        <v>20</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
         <v>114</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>114</v>
       </c>
-      <c r="E81" t="s">
-        <v>26</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="E83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" t="s">
-        <v>20</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
         <v>115</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>115</v>
       </c>
-      <c r="E82" t="s">
-        <v>26</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E84" t="s">
+        <v>26</v>
+      </c>
+      <c r="F84" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
         <v>116</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>116</v>
       </c>
-      <c r="E83" t="s">
-        <v>26</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E85" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="s">
-        <v>20</v>
-      </c>
-      <c r="B84" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
         <v>117</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>117</v>
       </c>
-      <c r="E84" t="s">
-        <v>26</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E86" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
         <v>118</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>118</v>
       </c>
-      <c r="E85" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E87" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
         <v>119</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>119</v>
       </c>
-      <c r="E86" t="s">
-        <v>26</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E88" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>204</v>
+      </c>
+      <c r="C89" t="s">
+        <v>204</v>
+      </c>
+      <c r="E89" t="s">
+        <v>26</v>
+      </c>
+      <c r="F89" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>205</v>
+      </c>
+      <c r="C90" t="s">
+        <v>205</v>
+      </c>
+      <c r="E90" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2842,18 +2934,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26171875" customWidth="1"/>
-    <col min="2" max="3" width="19.578125" customWidth="1"/>
-    <col min="4" max="4" width="13.68359375" customWidth="1"/>
-    <col min="5" max="7" width="11.68359375" customWidth="1"/>
-    <col min="8" max="8" width="19.578125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="39" customWidth="1"/>
-    <col min="10" max="13" width="11.68359375" customWidth="1"/>
+    <col min="10" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2888,7 +2980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -2923,7 +3015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
fixed retail indicators in union
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/53_Inst_Analysis_Unit_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/53_Inst_Analysis_Unit_RETAIL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="228">
   <si>
     <t>Analysis_Unit</t>
   </si>
@@ -717,6 +717,18 @@
   </si>
   <si>
     <t>RETAIL_IND_900</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_19</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_RETAIL_IND_20</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_19</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_20</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,16 +1779,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,16 +1796,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,16 +1813,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,16 +1830,16 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1835,16 +1847,16 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,16 +1864,16 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1869,16 +1881,16 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1886,16 +1898,16 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>198</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>198</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>200</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1903,16 +1915,16 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>199</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>201</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1920,16 +1932,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1937,16 +1949,16 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1954,16 +1966,16 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,16 +1983,16 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1988,16 +2000,16 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,16 +2017,16 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,16 +2034,16 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E35" t="s">
         <v>26</v>
       </c>
       <c r="F35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,16 +2051,16 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
       </c>
       <c r="F36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,16 +2068,16 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E37" t="s">
         <v>26</v>
       </c>
       <c r="F37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2073,16 +2085,16 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E38" t="s">
         <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,16 +2102,16 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E39" t="s">
         <v>26</v>
       </c>
       <c r="F39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,16 +2119,16 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E40" t="s">
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,16 +2136,16 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E41" t="s">
         <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2141,16 +2153,16 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E42" t="s">
         <v>26</v>
       </c>
       <c r="F42" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2158,16 +2170,16 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E43" t="s">
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,16 +2187,16 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E44" t="s">
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2192,16 +2204,16 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E45" t="s">
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2209,16 +2221,16 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="E46" t="s">
         <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2226,16 +2238,16 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="E47" t="s">
         <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2243,16 +2255,16 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="E48" t="s">
         <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2260,16 +2272,16 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E49" t="s">
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,16 +2289,16 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2294,16 +2306,16 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C51" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2311,16 +2323,16 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>216</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
+        <v>216</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,16 +2340,16 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="E53" t="s">
         <v>26</v>
       </c>
       <c r="F53" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2345,16 +2357,16 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E54" t="s">
         <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2362,16 +2374,16 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="E55" t="s">
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>123</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2379,16 +2391,16 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E56" t="s">
         <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,16 +2408,16 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E57" t="s">
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2413,16 +2425,16 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E58" t="s">
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,16 +2442,16 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E59" t="s">
         <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2447,16 +2459,16 @@
         <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E60" t="s">
         <v>26</v>
       </c>
       <c r="F60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2464,16 +2476,16 @@
         <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E61" t="s">
         <v>26</v>
       </c>
       <c r="F61" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,16 +2493,16 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E62" t="s">
         <v>26</v>
       </c>
       <c r="F62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,16 +2510,16 @@
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E63" t="s">
         <v>26</v>
       </c>
       <c r="F63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,16 +2527,16 @@
         <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E64" t="s">
         <v>26</v>
       </c>
       <c r="F64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2532,16 +2544,16 @@
         <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
         <v>26</v>
       </c>
       <c r="F65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2549,16 +2561,16 @@
         <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E66" t="s">
         <v>26</v>
       </c>
       <c r="F66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,16 +2578,16 @@
         <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E67" t="s">
         <v>26</v>
       </c>
       <c r="F67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2583,16 +2595,16 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E68" t="s">
         <v>26</v>
       </c>
       <c r="F68" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2600,16 +2612,16 @@
         <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E69" t="s">
         <v>26</v>
       </c>
       <c r="F69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2617,16 +2629,16 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E70" t="s">
         <v>26</v>
       </c>
       <c r="F70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2634,16 +2646,16 @@
         <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E71" t="s">
         <v>26</v>
       </c>
       <c r="F71" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2651,16 +2663,16 @@
         <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E72" t="s">
         <v>26</v>
       </c>
       <c r="F72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2668,16 +2680,16 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E73" t="s">
         <v>26</v>
       </c>
       <c r="F73" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,16 +2697,16 @@
         <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E74" t="s">
         <v>26</v>
       </c>
       <c r="F74" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2702,16 +2714,16 @@
         <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E75" t="s">
         <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,16 +2731,16 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E76" t="s">
         <v>26</v>
       </c>
       <c r="F76" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2736,16 +2748,16 @@
         <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E77" t="s">
         <v>26</v>
       </c>
       <c r="F77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2753,16 +2765,16 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E78" t="s">
         <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2770,16 +2782,16 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E79" t="s">
         <v>26</v>
       </c>
       <c r="F79" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2787,16 +2799,16 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E80" t="s">
         <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2804,16 +2816,16 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E81" t="s">
         <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2821,16 +2833,16 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E82" t="s">
         <v>26</v>
       </c>
       <c r="F82" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2838,16 +2850,16 @@
         <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E83" t="s">
         <v>26</v>
       </c>
       <c r="F83" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2855,16 +2867,16 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E84" t="s">
         <v>26</v>
       </c>
       <c r="F84" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2872,16 +2884,16 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E85" t="s">
         <v>26</v>
       </c>
       <c r="F85" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2889,16 +2901,16 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E86" t="s">
         <v>26</v>
       </c>
       <c r="F86" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2906,16 +2918,16 @@
         <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E87" t="s">
         <v>26</v>
       </c>
       <c r="F87" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2923,16 +2935,16 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E88" t="s">
         <v>26</v>
       </c>
       <c r="F88" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2940,16 +2952,16 @@
         <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E89" t="s">
         <v>26</v>
       </c>
       <c r="F89" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2957,16 +2969,16 @@
         <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C90" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E90" t="s">
         <v>26</v>
       </c>
       <c r="F90" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2974,16 +2986,16 @@
         <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>218</v>
+        <v>115</v>
       </c>
       <c r="C91" t="s">
-        <v>218</v>
+        <v>115</v>
       </c>
       <c r="E91" t="s">
         <v>26</v>
       </c>
       <c r="F91" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2991,16 +3003,16 @@
         <v>20</v>
       </c>
       <c r="B92" t="s">
-        <v>220</v>
+        <v>116</v>
       </c>
       <c r="C92" t="s">
-        <v>220</v>
+        <v>116</v>
       </c>
       <c r="E92" t="s">
         <v>26</v>
       </c>
       <c r="F92" t="s">
-        <v>221</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3008,16 +3020,16 @@
         <v>20</v>
       </c>
       <c r="B93" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="C93" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="E93" t="s">
         <v>26</v>
       </c>
       <c r="F93" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,16 +3037,16 @@
         <v>20</v>
       </c>
       <c r="B94" t="s">
-        <v>118</v>
+        <v>220</v>
       </c>
       <c r="C94" t="s">
-        <v>118</v>
+        <v>220</v>
       </c>
       <c r="E94" t="s">
         <v>26</v>
       </c>
       <c r="F94" t="s">
-        <v>160</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,16 +3054,16 @@
         <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C95" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E95" t="s">
         <v>26</v>
       </c>
       <c r="F95" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3059,16 +3071,16 @@
         <v>20</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>118</v>
       </c>
       <c r="C96" t="s">
-        <v>204</v>
+        <v>118</v>
       </c>
       <c r="E96" t="s">
         <v>26</v>
       </c>
       <c r="F96" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3076,16 +3088,16 @@
         <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="C97" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="E97" t="s">
         <v>26</v>
       </c>
       <c r="F97" t="s">
-        <v>207</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3093,15 +3105,49 @@
         <v>20</v>
       </c>
       <c r="B98" t="s">
+        <v>204</v>
+      </c>
+      <c r="C98" t="s">
+        <v>204</v>
+      </c>
+      <c r="E98" t="s">
+        <v>26</v>
+      </c>
+      <c r="F98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>205</v>
+      </c>
+      <c r="C99" t="s">
+        <v>205</v>
+      </c>
+      <c r="E99" t="s">
+        <v>26</v>
+      </c>
+      <c r="F99" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" t="s">
         <v>222</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C100" t="s">
         <v>222</v>
       </c>
-      <c r="E98" t="s">
-        <v>26</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F100" t="s">
         <v>223</v>
       </c>
     </row>

</xml_diff>